<commit_message>
Revised ClassID and added more detail internally for checking
</commit_message>
<xml_diff>
--- a/3 Resources/Legend.xlsx
+++ b/3 Resources/Legend.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EXploringEA\Documents\GitHub\EAII\3 Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EXploringEA\source\repos\EAInstallationInspector\3 Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC2C8940-AE58-4ECC-8A63-9021982C5646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B40F811E-5E54-4DFA-8ADD-5567A9F63602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8640" yWindow="2160" windowWidth="23880" windowHeight="12840" xr2:uid="{50036DC5-DA4C-4B65-AE75-D7B023A9BF71}"/>
+    <workbookView xWindow="-26655" yWindow="2940" windowWidth="23865" windowHeight="15135" xr2:uid="{50036DC5-DA4C-4B65-AE75-D7B023A9BF71}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">Sparx key doesn’t exist i.e., there is no classname specified for the key </t>
   </si>
@@ -51,6 +51,33 @@
   </si>
   <si>
     <t>Sparx key exists but No Class ID is set for the AddIn, hence the DLL cannot be identified</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sparx key exist and Class ID - Mismatch on AddIn name </t>
+  </si>
+  <si>
+    <t>FF0000</t>
+  </si>
+  <si>
+    <t>FF69B4</t>
+  </si>
+  <si>
+    <t>F5DE83</t>
+  </si>
+  <si>
+    <t>98FB98</t>
+  </si>
+  <si>
+    <t>FFFF00</t>
+  </si>
+  <si>
+    <t>FFC0CB</t>
+  </si>
+  <si>
+    <t>00FF00</t>
+  </si>
+  <si>
+    <t>Sparx key exist and Class ID - DLL does not appear to be a normal AddIn (integration?)</t>
   </si>
 </sst>
 </file>
@@ -73,7 +100,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -107,6 +134,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF5DEB3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF98FB98"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -138,7 +177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -153,6 +192,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -161,13 +206,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF98FB98"/>
+      <color rgb="FFFFFF00"/>
+      <color rgb="FFBCEEFA"/>
+      <color rgb="FFC8BCFA"/>
+      <color rgb="FFFFEBEE"/>
       <color rgb="FFF5DEB3"/>
       <color rgb="FF00FF00"/>
       <color rgb="FFFF0000"/>
       <color rgb="FFFF69B4"/>
       <color rgb="FFFFC0CB"/>
-      <color rgb="FFFFB7B7"/>
-      <color rgb="FFFFDBB7"/>
     </mruColors>
   </colors>
   <extLst>
@@ -478,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A12378BD-A710-4489-89F5-205112283FD0}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection sqref="A1:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,29 +537,60 @@
     <col min="1" max="1" width="87.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="4" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="5" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working version updated: *  present more information in pop-ip dialog with entry details of AddIn Class and CLSID class * change the colours to make less dramatic
</commit_message>
<xml_diff>
--- a/3 Resources/Legend.xlsx
+++ b/3 Resources/Legend.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EXploringEA\source\repos\EAInstallationInspector\3 Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B40F811E-5E54-4DFA-8ADD-5567A9F63602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C806DA7-A027-4961-8A85-0B6A982B0D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26655" yWindow="2940" windowWidth="23865" windowHeight="15135" xr2:uid="{50036DC5-DA4C-4B65-AE75-D7B023A9BF71}"/>
+    <workbookView xWindow="-26775" yWindow="7530" windowWidth="23865" windowHeight="15135" xr2:uid="{50036DC5-DA4C-4B65-AE75-D7B023A9BF71}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t xml:space="preserve">Sparx key doesn’t exist i.e., there is no classname specified for the key </t>
   </si>
@@ -62,15 +62,6 @@
     <t>FF69B4</t>
   </si>
   <si>
-    <t>F5DE83</t>
-  </si>
-  <si>
-    <t>98FB98</t>
-  </si>
-  <si>
-    <t>FFFF00</t>
-  </si>
-  <si>
     <t>FFC0CB</t>
   </si>
   <si>
@@ -78,6 +69,18 @@
   </si>
   <si>
     <t>Sparx key exist and Class ID - DLL does not appear to be a normal AddIn (integration?)</t>
+  </si>
+  <si>
+    <t>BAFCBA</t>
+  </si>
+  <si>
+    <t>Can't exist!</t>
+  </si>
+  <si>
+    <t>E8FEE8</t>
+  </si>
+  <si>
+    <t>FFE699</t>
   </si>
 </sst>
 </file>
@@ -133,19 +136,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF5DEB3"/>
+        <fgColor rgb="FF90FA90"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFE8FEE8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF98FB98"/>
+        <fgColor rgb="FFFFE699"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -182,9 +185,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -192,6 +192,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -206,16 +209,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
-      <color rgb="FF98FB98"/>
-      <color rgb="FFFFFF00"/>
-      <color rgb="FFBCEEFA"/>
-      <color rgb="FFC8BCFA"/>
-      <color rgb="FFFFEBEE"/>
-      <color rgb="FFF5DEB3"/>
-      <color rgb="FF00FF00"/>
-      <color rgb="FFFF0000"/>
-      <color rgb="FFFF69B4"/>
-      <color rgb="FFFFC0CB"/>
+      <color rgb="FFFFE699"/>
+      <color rgb="FFE8FEE8"/>
+      <color rgb="FF90FA90"/>
+      <color rgb="FF62F862"/>
+      <color rgb="FFCCFCCC"/>
+      <color rgb="FFB3FBBF"/>
+      <color rgb="FFFFFF66"/>
+      <color rgb="FFFFFF99"/>
+      <color rgb="FFEBFAB4"/>
+      <color rgb="FFBAFCBA"/>
     </mruColors>
   </colors>
   <extLst>
@@ -526,71 +529,144 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A12378BD-A710-4489-89F5-205112283FD0}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A7"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="87.7109375" customWidth="1"/>
+    <col min="2" max="2" width="87.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1">
+        <v>0</v>
+      </c>
+      <c r="G1">
+        <v>255</v>
+      </c>
+      <c r="H1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2">
+        <v>186</v>
+      </c>
+      <c r="G2">
+        <v>252</v>
+      </c>
+      <c r="H2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3">
+        <v>232</v>
+      </c>
+      <c r="G3">
+        <v>254</v>
+      </c>
+      <c r="H3">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4">
+        <v>255</v>
+      </c>
+      <c r="G4">
+        <v>230</v>
+      </c>
+      <c r="H4">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5">
+        <v>255</v>
+      </c>
+      <c r="G5">
+        <v>192</v>
+      </c>
+      <c r="H5">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6">
+        <v>255</v>
+      </c>
+      <c r="G6">
+        <v>105</v>
+      </c>
+      <c r="H6">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11">
+        <v>255</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="J11" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>